<commit_message>
Added ExcelVBA for AutoFitting columns
</commit_message>
<xml_diff>
--- a/GeneratedReport.xlsx
+++ b/GeneratedReport.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rah/PycharmProjects/xStackExport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA6052E-11B0-8D47-934B-83047BAC4077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CF1F87-DB57-B542-B5DD-721286DC09B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="33360" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="33140" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exported" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,9 @@
     <t>Department of Information Technology</t>
   </si>
   <si>
+    <t>Student attendance for the period: Apr 1, 2020 to May 1, 2020</t>
+  </si>
+  <si>
     <t>Registration #</t>
   </si>
   <si>
@@ -53,19 +56,23 @@
   </si>
   <si>
     <t>z</t>
-  </si>
-  <si>
-    <t>Student attendance for the period: Apr 1, 2020 to May 1, 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,7 +87,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF800080"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -123,7 +130,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -470,26 +477,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="218" workbookViewId="0">
       <selection sqref="A1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -553,7 +548,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -583,25 +578,25 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -611,40 +606,40 @@
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="J5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="N5" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>